<commit_message>
Fixed incorrect filling of columns with unique values for the case columns>1
</commit_message>
<xml_diff>
--- a/Parameters/ShortDivisionNames.xlsx
+++ b/Parameters/ShortDivisionNames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ddd\04. Настройки\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DES.LM.Reports\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDBF27B-557F-4417-97A5-DA3159E88CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B209E10-7FE2-4858-9B4F-5F9EABEACA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Администрация</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Направление информационных систем</t>
   </si>
   <si>
-    <t>НИС</t>
-  </si>
-  <si>
     <t>НПИС</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Направление систем промышленной безопасности и экологии</t>
   </si>
   <si>
-    <t>Направление СПБиЭ</t>
-  </si>
-  <si>
     <t>Служба развития бизнеса</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Служба управления производством</t>
   </si>
   <si>
-    <t>СУП</t>
-  </si>
-  <si>
     <t>FullDivisionName</t>
   </si>
   <si>
@@ -106,18 +97,44 @@
   </si>
   <si>
     <t>Направление поддержки информационных систем</t>
+  </si>
+  <si>
+    <t>Отдел обеспечения деятельности</t>
+  </si>
+  <si>
+    <t>СУП+ООД</t>
+  </si>
+  <si>
+    <t>Отдел научно-исследовательских разработок</t>
+  </si>
+  <si>
+    <t>СРБ Отдел НИР</t>
+  </si>
+  <si>
+    <t>Отдел поддержки</t>
+  </si>
+  <si>
+    <t>(прочие)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -151,23 +168,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{57EEE6B0-97DE-4F04-B9AB-A0C51B012999}"/>
+    <cellStyle name="Обычный 3 2" xfId="3" xr:uid="{D6806773-A4BB-4F42-A809-CA6EA8475A14}"/>
+    <cellStyle name="Процентный 2" xfId="2" xr:uid="{0AD39554-FAB6-473D-8E10-8C6B612BC0C5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,11 +467,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F53492B-E9B6-44FD-A10D-37455B40CAC6}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -460,13 +480,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -507,7 +527,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>-3</v>
@@ -515,10 +535,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2">
         <v>-1</v>
@@ -526,10 +546,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>165</v>
@@ -537,10 +557,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C8" s="2">
         <v>-2</v>
@@ -548,10 +568,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C9" s="2">
         <v>159</v>
@@ -559,10 +579,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2">
         <v>-4</v>
@@ -570,10 +590,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
         <v>154</v>
@@ -581,29 +601,47 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2">
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+    <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2">
+        <v>154</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2">
+        <v>154</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -665,8 +703,12 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bjpfJLEDoVgNseqSdbqmB2CAjCIwC8LB3Xh7qg+4/UEPTj9NlELs8Y1kgTnExXjK6OyaKjBp/HyWc1DvsV4wGw==" saltValue="54cu2JcQ9rQmmQVfw9BLRQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Some changes in reports
The attribute "vacancy" has been added.
A new report has been added to check planned indicators.
Changed settings.
</commit_message>
<xml_diff>
--- a/Parameters/ShortDivisionNames.xlsx
+++ b/Parameters/ShortDivisionNames.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26993244-EE3B-4C5A-8E24-5EFC566DEEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A025AC40-AD41-49F8-8A7D-F80A3FBB514C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Администрация</t>
   </si>
@@ -103,13 +103,16 @@
     <t>Отдел научно-исследовательских разработок</t>
   </si>
   <si>
-    <t>СРБ Отдел НИР</t>
-  </si>
-  <si>
     <t>Отдел поддержки</t>
   </si>
   <si>
     <t>(прочие)</t>
+  </si>
+  <si>
+    <t>ДОР.ОП</t>
+  </si>
+  <si>
+    <t>Отдел НИР</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F53492B-E9B6-44FD-A10D-37455B40CAC6}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -522,7 +527,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
         <v>-3</v>
@@ -577,7 +582,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2">
         <v>-4</v>
@@ -621,7 +626,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2">
         <v>154</v>
@@ -629,10 +634,10 @@
     </row>
     <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2">
         <v>154</v>

</xml_diff>